<commit_message>
Updating Old File for core commit 4466579475a16d07150b9504d338a8c4a873ab8b
</commit_message>
<xml_diff>
--- a/help/interface/data-collection/cookies/assets/First_Party_Domain_Request_Form.xlsx
+++ b/help/interface/data-collection/cookies/assets/First_Party_Domain_Request_Form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgrover/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfrei\Documents\Git\core-services.en\help\interface\data-collection\cookies\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A65731CD-E668-FF4F-AD7A-CE1A518195A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B14DE0-A007-4430-A579-AA4BBC6A558A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="51200" windowHeight="28340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPC Request Form" sheetId="1" r:id="rId1"/>
@@ -149,9 +149,6 @@
     <t>Fill in all required fields in the form below (see sample for reference)</t>
   </si>
   <si>
-    <t>Forward this request form to clientcare@adobe.com</t>
-  </si>
-  <si>
     <t>Adobe purchases and applies certificate during the next available maintenance window</t>
   </si>
   <si>
@@ -208,6 +205,7 @@
         <sz val="14"/>
         <color theme="5"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Optional</t>
@@ -217,6 +215,7 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
@@ -231,6 +230,7 @@
         <sz val="14"/>
         <color theme="5"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Optional</t>
@@ -240,6 +240,7 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
@@ -252,9 +253,6 @@
     <t>Certificate Management</t>
   </si>
   <si>
-    <t>Adobe will purchase and maintain your certificate during each subsequent renewal cycle.  Exemptions to the Adobe Managed Certificate Program can be submitted to clientcare@adobe.com for consideration and approval.</t>
-  </si>
-  <si>
     <t>California</t>
   </si>
   <si>
@@ -264,9 +262,6 @@
     <t>telemetry.adobe.com</t>
   </si>
   <si>
-    <t>Update CNAME to point to Adobe Hostnames that will be provided by Client Care</t>
-  </si>
-  <si>
     <t>certs@adobe.com</t>
   </si>
   <si>
@@ -277,13 +272,66 @@
   </si>
   <si>
     <t xml:space="preserve">The CNAME you create can be used for both Analytics and the Edge Network (WebSDK).  </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a Support case in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Admin Console</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Support</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and attach the file to that ticket</t>
+    </r>
+  </si>
+  <si>
+    <t>Adobe will purchase and maintain your certificate during each subsequent renewal cycle.  Exemptions to the Adobe Managed Certificate Program can be submitted to Adobe for consideration and approval.</t>
+  </si>
+  <si>
+    <t>Update CNAME to point to Adobe Hostnames that will be provided by Support</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -295,12 +343,14 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -324,12 +374,14 @@
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="5"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -337,6 +389,7 @@
       <sz val="14"/>
       <color theme="5"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -349,6 +402,7 @@
       <sz val="18"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -388,6 +442,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -596,9 +658,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -608,118 +670,115 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1068,11 +1127,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="B22:L23"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="2" width="4.33203125" customWidth="1"/>
     <col min="3" max="5" width="15.83203125" customWidth="1"/>
@@ -1080,24 +1139,24 @@
     <col min="12" max="13" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="40"/>
-    </row>
-    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="23.35" x14ac:dyDescent="0.8">
+      <c r="A1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="20"/>
+    </row>
+    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1112,100 +1171,100 @@
       <c r="L2" s="7"/>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A3" s="6"/>
-      <c r="B3" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="36"/>
+      <c r="B3" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="29"/>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A4" s="6"/>
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="38"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="31"/>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A5" s="6"/>
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="31"/>
+      <c r="C5" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="33"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A6" s="6"/>
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="31"/>
+      <c r="C6" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="33"/>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A7" s="6"/>
       <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="33"/>
+      <c r="C7" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="35"/>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1220,32 +1279,32 @@
       <c r="L8" s="7"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
+      <c r="C9" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="18"/>
+      <c r="J9" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="36"/>
       <c r="L9" s="5"/>
       <c r="M9" s="9"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -1253,183 +1312,183 @@
       <c r="G10" s="25"/>
       <c r="H10" s="26"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="28"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
       <c r="L10" s="5"/>
       <c r="M10" s="9"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
+      <c r="C11" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="19"/>
+      <c r="J11" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="21"/>
       <c r="L11" s="7"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
+      <c r="C12" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="19"/>
+      <c r="J12" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="21"/>
       <c r="L12" s="7"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+      <c r="C13" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="19"/>
+      <c r="J13" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="21"/>
       <c r="L13" s="7"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
-      <c r="C14" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
+      <c r="C14" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="19"/>
+      <c r="J14" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="21"/>
       <c r="L14" s="7"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
+      <c r="C15" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="19"/>
+      <c r="J15" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="21"/>
       <c r="L15" s="7"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
+      <c r="C16" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="K16" s="42"/>
+      <c r="J16" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="23"/>
       <c r="L16" s="7"/>
       <c r="M16" s="8"/>
     </row>
-    <row r="17" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
+      <c r="C17" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
       <c r="L17" s="7"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
+      <c r="C18" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="19"/>
+      <c r="J18" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="21"/>
       <c r="L18" s="7"/>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
+      <c r="C19" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="19"/>
+      <c r="J19" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="21"/>
       <c r="L19" s="7"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1444,62 +1503,62 @@
       <c r="L20" s="7"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A21" s="6"/>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A22" s="6"/>
+      <c r="B22" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="8"/>
-    </row>
-    <row r="22" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A23" s="6"/>
-      <c r="B23" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="46"/>
+      <c r="B23" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="17"/>
       <c r="M23" s="8"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -1516,6 +1575,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:L22"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="J14:K14"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="E23:L23"/>
     <mergeCell ref="A1:M1"/>
@@ -1532,31 +1616,6 @@
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:L22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>